<commit_message>
Đức test lại menu,
</commit_message>
<xml_diff>
--- a/Services/Server/Server.API/wwwroot/Reports/DANHSACHHOCSINH.xlsx
+++ b/Services/Server/Server.API/wwwroot/Reports/DANHSACHHOCSINH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACS\KhachHang\AMMS_DiemDanhHocSinh\Services\Server\Server.API\wwwroot\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEBBCCC-FF83-4084-92DB-BADA2BFBF40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3502A098-3974-48E3-AB14-9AD64DDAAB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>{{item.FullName}}</t>
   </si>
   <si>
-    <t>{{item.IsFace}}</t>
-  </si>
-  <si>
     <t>{{item.SyncCode}}</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Mã CSDLN</t>
+  </si>
+  <si>
+    <t>{{item.IsFaceName}}</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -765,7 +765,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>18</v>
@@ -790,19 +790,19 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="L7" s="1"/>
     </row>

</xml_diff>